<commit_message>
added rdf and updated script, removed imgs
</commit_message>
<xml_diff>
--- a/fotolijsten/Fotolijst_Dongeradeel.xlsx
+++ b/fotolijsten/Fotolijst_Dongeradeel.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="67">
   <si>
     <t>Bewaarplaats</t>
   </si>
@@ -217,27 +217,6 @@
   </si>
   <si>
     <t>Let op: op de originelen staat geen nummering. De nummering is op grond van de volgorde in de map</t>
-  </si>
-  <si>
-    <t>Brief van de reder aan de waterschout betreffend aanmonstering op de KW 39 Doggersbank</t>
-  </si>
-  <si>
-    <t>Machtiging van de reder aan de schipper betreffend aanmonstering op de KW 39 Doggersbank</t>
-  </si>
-  <si>
-    <t>Machtiging van de reder aan de schipper betreffend aanmonstering op de KW 158</t>
-  </si>
-  <si>
-    <t>De in de volmacht genoemde schepen staan niet in de monsterrollendatabase door ontbreken van de monsterrol</t>
-  </si>
-  <si>
-    <t>1916-6 en 8</t>
-  </si>
-  <si>
-    <t>Briefjes van ouders en verder een machtiging van de schipper aan L. Akkerman om bemanningsleden te werven</t>
-  </si>
-  <si>
-    <t>Geen specifiek schip genoemd,dus niet te linken.</t>
   </si>
 </sst>
 </file>
@@ -584,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J455"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -597,9 +576,9 @@
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="84.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="103.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="93.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -662,54 +641,36 @@
         <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G4" t="s">
         <v>49</v>
       </c>
-      <c r="H4" t="s">
-        <v>53</v>
-      </c>
       <c r="I4" s="3"/>
-      <c r="J4" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="E5" t="s">
         <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G5" t="s">
         <v>45</v>
       </c>
-      <c r="H5" t="s">
-        <v>53</v>
-      </c>
       <c r="I5" s="3"/>
-      <c r="J5" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="E6" t="s">
         <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G6" t="s">
         <v>45</v>
       </c>
-      <c r="H6" t="s">
-        <v>57</v>
-      </c>
       <c r="I6" s="3"/>
-      <c r="J6" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="E7" t="s">
@@ -722,22 +683,16 @@
         <v>46</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="E8" t="s">
         <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G8" t="s">
         <v>47</v>
-      </c>
-      <c r="H8" t="s">
-        <v>71</v>
       </c>
       <c r="I8" s="3"/>
     </row>
@@ -746,18 +701,12 @@
         <v>22</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G9" t="s">
         <v>48</v>
       </c>
-      <c r="H9" t="s">
-        <v>57</v>
-      </c>
       <c r="I9" s="3"/>
-      <c r="J9" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="E10" t="s">
@@ -770,9 +719,6 @@
         <v>49</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="E11" t="s">

</xml_diff>